<commit_message>
Documentos inclusos [Jornal e outros]
</commit_message>
<xml_diff>
--- a/Documentos/Plano de Ação.xlsx
+++ b/Documentos/Plano de Ação.xlsx
@@ -138,7 +138,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Documentação, 
+      <t xml:space="preserve">Documentação e Back-End
 </t>
     </r>
     <r>
@@ -859,8 +859,8 @@
   </sheetPr>
   <dimension ref="B1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I10" activeCellId="0" sqref="I10"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1123,8 +1123,8 @@
       <c r="G14" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="H14" s="35" t="s">
-        <v>28</v>
+      <c r="H14" s="32" t="s">
+        <v>24</v>
       </c>
       <c r="I14" s="31" t="s">
         <v>38</v>

</xml_diff>